<commit_message>
---- Ajout Fichier Excel ---
</commit_message>
<xml_diff>
--- a/Consolidation_Evaluation.xlsx
+++ b/Consolidation_Evaluation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Vous avez réussi à accomplir la tâche 1</t>
   </si>
@@ -96,6 +96,27 @@
   </si>
   <si>
     <t>Consolidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tâche 1 : </t>
+  </si>
+  <si>
+    <t>Tâche 3 :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tâche 2 : </t>
+  </si>
+  <si>
+    <t>Réserver un cours</t>
+  </si>
+  <si>
+    <t>Rechercher de nouveaux tournois</t>
+  </si>
+  <si>
+    <t>Regarder des photos des évènements passés</t>
   </si>
 </sst>
 </file>
@@ -587,19 +608,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.95" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -613,237 +638,224 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>4</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
         <f>IF(AND(C2=0,D2=0,B2=0),0,(B2+C2+D2)/((IF(B2=0,0,1)+IF(C2=0,0,1)+IF(D2=0,0,1))))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E22" si="0">IF(AND(C3=0,D3=0,B3=0),0,(B3+C3+D3)/((IF(B3=0,0,1)+IF(C3=0,0,1)+IF(D3=0,0,1))))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
-        <v>2</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
-        <v>2</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
-        <v>2</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
-        <v>2</v>
-      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4">
-        <v>2</v>
-      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
-        <v>0</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
@@ -855,56 +867,48 @@
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
-        <v>2</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
-        <v>3</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4">
-        <v>3</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
--- Ebauche rapport ---
</commit_message>
<xml_diff>
--- a/Consolidation_Evaluation.xlsx
+++ b/Consolidation_Evaluation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Vous avez réussi à accomplir la tâche 1</t>
   </si>
@@ -110,13 +110,28 @@
     <t xml:space="preserve">Tâche 2 : </t>
   </si>
   <si>
-    <t>Réserver un cours</t>
-  </si>
-  <si>
-    <t>Rechercher de nouveaux tournois</t>
-  </si>
-  <si>
-    <t>Regarder des photos des évènements passés</t>
+    <t>Trouver un stage pour les vacances</t>
+  </si>
+  <si>
+    <t>Connaitre les documents nécessaire à l'inscription de sa fille ainsi que le règlement du club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regarder pour trouver un cours pour sa fille </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points Faibles : </t>
+  </si>
+  <si>
+    <t>Travail de mémorisation</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Audience non déterminée</t>
+  </si>
+  <si>
+    <t>Objectif divers et peu clairs (la plupart non complet)</t>
   </si>
 </sst>
 </file>
@@ -132,15 +147,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -224,11 +245,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -248,6 +320,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.95" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -620,8 +700,8 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -642,273 +722,379 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
         <f>IF(AND(C2=0,D2=0,B2=0),0,(B2+C2+D2)/((IF(B2=0,0,1)+IF(C2=0,0,1)+IF(D2=0,0,1))))</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
-        <v>29</v>
+      <c r="H2" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E22" si="0">IF(AND(C3=0,D3=0,B3=0),0,(B3+C3+D3)/((IF(B3=0,0,1)+IF(C3=0,0,1)+IF(D3=0,0,1))))</f>
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
-        <v>30</v>
+      <c r="H3" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
-        <v>31</v>
+      <c r="H4" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>4</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="6">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="4">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="4">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="4">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="6">
+        <v>3</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
--- Avancée suite au cours du 07/12/2016 ---
</commit_message>
<xml_diff>
--- a/Consolidation_Evaluation.xlsx
+++ b/Consolidation_Evaluation.xlsx
@@ -13,8 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -122,16 +121,16 @@
     <t xml:space="preserve">Points Faibles : </t>
   </si>
   <si>
-    <t>Travail de mémorisation</t>
-  </si>
-  <si>
     <t>Navigation</t>
   </si>
   <si>
-    <t>Audience non déterminée</t>
-  </si>
-  <si>
-    <t>Objectif divers et peu clairs (la plupart non complet)</t>
+    <t>Design, processus et évaluation</t>
+  </si>
+  <si>
+    <t>Lien</t>
+  </si>
+  <si>
+    <t>Optimiser l'expérience de l'utilisateur</t>
   </si>
 </sst>
 </file>
@@ -690,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.95" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -701,7 +700,7 @@
     <col min="4" max="4" width="11.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -822,7 +821,7 @@
         <v>32</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -842,7 +841,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -862,7 +861,7 @@
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1153,16 +1152,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>